<commit_message>
Ecriture de bombe.js / Mise à jour des tâches Mise en place pas encore effectué dans le main Disfonctionnement normal ;)
</commit_message>
<xml_diff>
--- a/taches.xlsx
+++ b/taches.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="46">
   <si>
     <t>TACHES</t>
   </si>
@@ -145,16 +145,31 @@
   </si>
   <si>
     <t xml:space="preserve">Création de Maps / Décors </t>
+  </si>
+  <si>
+    <t>Definir règles de nommages / code</t>
+  </si>
+  <si>
+    <t>PROGRESSION (%)</t>
+  </si>
+  <si>
+    <t>undefined</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -219,7 +234,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -227,6 +242,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -528,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -540,10 +562,11 @@
     <col min="2" max="2" width="76.7109375" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
     <col min="4" max="4" width="13.85546875" customWidth="1"/>
-    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -557,10 +580,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -571,11 +597,14 @@
       <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -586,11 +615,14 @@
       <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -601,11 +633,14 @@
       <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>18</v>
       </c>
@@ -618,174 +653,226 @@
       <c r="D5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="8">
+        <v>0</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C7" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>16</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E7" s="8">
+        <v>0</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8" s="2"/>
+        <v>15</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="C8" s="3" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="8">
+        <v>0</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="8">
+        <v>0</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B10" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3" t="s">
-        <v>33</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="8">
+        <v>0</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="8">
+        <v>0</v>
+      </c>
+      <c r="F11" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>30</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="8">
+        <v>0</v>
+      </c>
+      <c r="F12" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="8">
+        <v>0</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C14" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>31</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="8">
+        <v>0</v>
+      </c>
+      <c r="F14" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="8">
+        <v>0</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B16" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E16" s="8">
+        <v>0</v>
+      </c>
+      <c r="F16" s="6" t="s">
         <v>25</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>